<commit_message>
rats test for pedroni causality
</commit_message>
<xml_diff>
--- a/test-results/Vargranger_results.xlsx
+++ b/test-results/Vargranger_results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caw6/Desktop/UrbanizationCauseConsequence/test-results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Desktop\UrbanizationCauseConsequence\test-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21160" windowHeight="17620" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="21165" windowHeight="17625" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GDPPerCapRealLCU_1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>Country</t>
   </si>
@@ -150,16 +150,22 @@
   </si>
   <si>
     <t>Belize</t>
+  </si>
+  <si>
+    <t>GDP -&gt; PctUrb chi2</t>
+  </si>
+  <si>
+    <t>PctUrb -&gt; GDP chi2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -201,6 +207,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -475,16 +484,16 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -518,7 +527,7 @@
         <v>6.9145976597441372E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -535,7 +544,7 @@
         <v>1.6553031549208512E-28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -552,7 +561,7 @@
         <v>4.269280757044952E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -569,7 +578,7 @@
         <v>0.11482234542107421</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -586,7 +595,7 @@
         <v>0.22984847733923625</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -603,7 +612,7 @@
         <v>8.4561953028473406E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -620,7 +629,7 @@
         <v>3.1776218561012877E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -637,7 +646,7 @@
         <v>1.6396839783930157E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -654,7 +663,7 @@
         <v>9.6742247948396372E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -671,7 +680,7 @@
         <v>2.9768947131828122E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -688,7 +697,7 @@
         <v>1.8903526915385053E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -705,7 +714,7 @@
         <v>8.5944196502155679E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -722,7 +731,7 @@
         <v>1.0527978741750191E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -739,7 +748,7 @@
         <v>0.10197823942135224</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -756,7 +765,7 @@
         <v>3.7968739586545387E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -773,7 +782,7 @@
         <v>0.91823861416084918</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -790,7 +799,7 @@
         <v>5.9281612824609023E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -807,7 +816,7 @@
         <v>0.47389680903151554</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -824,7 +833,7 @@
         <v>3.1230643981088307E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -841,7 +850,7 @@
         <v>0.50802673574366186</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -858,7 +867,7 @@
         <v>1.4373108531938526E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -891,16 +900,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -917,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -934,7 +943,7 @@
         <v>6.9145864734614773E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -951,7 +960,7 @@
         <v>1.6551288620674052E-28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -968,7 +977,7 @@
         <v>0.32017030520815265</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -985,7 +994,7 @@
         <v>1.6082834980301271E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>0.81887624017161609</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1028,7 @@
         <v>0.18361854912748413</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>3.1776216151676037E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>0.14573810370465767</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>4.4848981415391903E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1096,7 @@
         <v>9.6742135172666888E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1104,7 +1113,7 @@
         <v>1.8162048458132043E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>1.0527975994344602E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>3.648511876179911E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>5.7617243467941474E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1188,15 +1197,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>0.16532563025249816</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1247,7 +1256,7 @@
         <v>6.9145864734614773E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>1.6551288620674052E-28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>4.6978945155838128E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>1.4947333923061763E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>2.363148296156652E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>3.1776216151676037E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>0.11515136321869272</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>8.6867094812761829E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1392,7 @@
         <v>9.6742135172666888E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>1.8162048458132043E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>1.5332160890220619E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1443,7 @@
         <v>1.0527975994344602E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1451,7 +1460,7 @@
         <v>0.13084190342238822</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>5.3020499009365469E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>1.2143859159617991E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>3.6156714385204651E-18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>1.3420668254474001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1549,35 +1558,35 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>2.0018993060144361E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>6.9145864734614773E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>1.6551288620674052E-28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>1.6082834980301271E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>0.81887624017161609</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>0.18361854912748413</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>3.1776216151676037E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>4.4848981415391903E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>9.6742135172666888E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>1.0527975994344602E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1764,7 +1773,7 @@
         <v>3.648511876179911E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1790,7 @@
         <v>3.7968881946747594E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
cum_Govt panel + graphs
</commit_message>
<xml_diff>
--- a/test-results/Vargranger_results.xlsx
+++ b/test-results/Vargranger_results.xlsx
@@ -9,28 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="21165" windowHeight="17625" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="21165" windowHeight="17625" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GDPPerCapRealLCU_1" sheetId="1" r:id="rId1"/>
     <sheet name="GDPPerCapRealLCU_2" sheetId="2" r:id="rId2"/>
     <sheet name="GDPPerCapRealUSD" sheetId="3" r:id="rId3"/>
     <sheet name="GDPRealLCU" sheetId="4" r:id="rId4"/>
+    <sheet name="cum_Govt" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Country</t>
   </si>
@@ -156,6 +149,105 @@
   </si>
   <si>
     <t>PctUrb -&gt; GDP chi2</t>
+  </si>
+  <si>
+    <t>cum_Govt -&gt; PctUrb chi2</t>
+  </si>
+  <si>
+    <t>PctUrb -&gt; cum_Govt chi2</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Venezuela, RB</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Zambia</t>
   </si>
 </sst>
 </file>
@@ -1557,12 +1649,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -1813,4 +1906,622 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2">
+        <v>116.76215944202019</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4.4199690634033109E-26</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.34583818699846536</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.84120567109876365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2">
+        <v>102.82456765729553</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.6981711229677782E-23</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.91289110816188934</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.63353150165939476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2">
+        <v>72.848306739473145</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.5177183448304706E-16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.7520501354159883</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.1531978481629567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2">
+        <v>57.667767402888558</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.0033325059937359E-13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3213564060092864</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.51650092320211916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2">
+        <v>34.854201293550467</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.7008866207920427E-8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.5557574889317376</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.10250140794329474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2">
+        <v>31.494989971924269</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.4486044793926115E-7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>46.942785548923027</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.4047714296395926E-11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2">
+        <v>27.582335438960968</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0246415442336814E-6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>28.815183225303155</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.5317489884523327E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2">
+        <v>27.38097097847583</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.1331768600113821E-6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.7694736027912539</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.41282281336979465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="2">
+        <v>27.170764617664418</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.258761434639437E-6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.8833481343333993</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.23653145751037502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2">
+        <v>26.869276699712142</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.4635605622856722E-6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.90522315802600506</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.63596510785321114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2">
+        <v>26.144564524249972</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.1027127479665662E-6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13.807594086856909</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.0039660797142953E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2">
+        <v>25.673171659319969</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.6615927673305031E-6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.3965071822470776</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.30172067973765798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2">
+        <v>24.692620705878198</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.3457580353237854E-6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>7.2792452694655054</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.626225255794614E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2">
+        <v>23.58713825133097</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7.5529742969390981E-6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>17.265878145246745</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.7814030770811067E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2">
+        <v>23.236393449968382</v>
+      </c>
+      <c r="C16" s="2">
+        <v>9.0008033366454049E-6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8.1998481286077318</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.6573933907186821E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2">
+        <v>22.671577096590852</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.1937945323158705E-5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.98842674022958565</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.61005060263575062</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2">
+        <v>20.793777586986835</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.0527312187638162E-5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10.959870633290805</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4.1695993928576895E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2">
+        <v>20.702486555494716</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.195303857009905E-5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.6948473049205717</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.42851752107360386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2">
+        <v>18.914386167846828</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7.812557546964244E-5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>24.372611479507981</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5.0998178235018482E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2">
+        <v>18.718253358557757</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8.6175324560002755E-5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>63.269179414885265</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.803034991941925E-15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="2">
+        <v>18.638809117306792</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8.9667286119957365E-5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5.1038460180008229</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7.793165853374763E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2">
+        <v>18.260168355724602</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.0835646349993803E-4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.5363892822702976</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.17064077874879652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2">
+        <v>16.94864016818542</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.0876108703626447E-4</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.10482523600859758</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.94893723746265257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="2">
+        <v>14.271995634081321</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7.9593119281712603E-4</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.26657350848911582</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.87521408476807683</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="2">
+        <v>13.583608427612489</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.1229409198723289E-3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.63779534152252149</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.72694993373374295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2">
+        <v>12.503677085764139</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.9269081742168443E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>30.53022997110736</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.346630959830227E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2">
+        <v>10.599318579386818</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4.9932948841544022E-3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>7.6034986398118489</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2.2331672428321174E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2">
+        <v>9.8994234423026199</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7.0854512203835408E-3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>20065.354695057918</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
+        <v>9.1280471924310405</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1.0420048416031827E-2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6.5352219702027394</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3.809733354091456E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="2">
+        <v>9.117718324576316</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.0474001265643495E-2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5.6312565516643787</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5.9867093873728426E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="2">
+        <v>5.9535474616641295</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5.0956969849810914E-2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5.1872356792345116</v>
+      </c>
+      <c r="E32" s="2">
+        <v>7.4749119980463088E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2">
+        <v>5.569942726813542</v>
+      </c>
+      <c r="C33" s="2">
+        <v>6.1730856767082627E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6.1803039765349244</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.5495039166936271E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.3169668414621327</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.31396196821904138</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.2516663199026326</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.1967476846071525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.40661535478068345</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.81602712969917668</v>
+      </c>
+      <c r="D35" s="2">
+        <v>12.184681559945659</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2.2601122925284003E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E35">
+    <sortCondition descending="1" ref="B2:B35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>